<commit_message>
Add all the policy proposals.
</commit_message>
<xml_diff>
--- a/Cited papers in NAIVETE-BASED DISCRIMINATION.xlsx
+++ b/Cited papers in NAIVETE-BASED DISCRIMINATION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergeimolinari/Desktop/RM Behavioral Contract Theory/research_module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB841E7-3428-9A4D-9DB2-20E3AF7F060B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865A8076-63E5-9742-927F-FD2DB88FF13E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4B174A89-2607-9749-ADDE-E0B6D10E6700}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="251">
   <si>
     <t>Authors</t>
   </si>
@@ -777,13 +777,39 @@
     <t>"Our analysis highlights an important dimension of the use of naiveté based discrimination that has been largely ignored in the literature. The interaction between behavioral screening and classic adverse selection is more complex than the prior theory literature has taken into account. There appears to be an inbuilt trade off between the immediate benefits from using naiveté based price discrimination and their impact on the credit risk of the customer pool. By drawing in customers who do not understand the credit terms that they are offered the issuer might end up with borrowers who have a higher chance that they can ultimately not afford the credit and default. The results in this paper provide evidence that credit card companies do target and screen sophisticated and naïve creditors differently, via the type of reward programs and pricing structures that are offered to customers. Issuers offer customers a menu of contracts to choose from; so rational customers on average can find contracts with less hidden charges. However naïve customers will also be able to find contracts that cater to their behavioral problems. But we can see that on average the menu of cards that is offered to more educated and richer customers contains fewer cards with hidden charges than the one offered to less educated and poorer customers. This means the latter group has to work harder to pick their card." -&gt; NO policy proposals though.</t>
   </si>
   <si>
-    <t>ALL THE PAPER IS SUPER INTEETING AND RELEVANT -&gt; "We analyze nine regulatory strategies that may help individuals avoid financial mistakes. We discuss laissez-faire, disclosure, nudges, financial “driver’s licenses,” advance directives, fiduciaries, asset safe harbors, and ex post and ex ante regulatory oversight. Finally, we pose seven questions for future research on cognitive limitations and associated policy responses."</t>
-  </si>
-  <si>
     <t>No access, but it suggests that merely having disclosure regulations in place is insufficient; robust enforcement mechanisms are crucial to ensure compliance and protect consumers.</t>
   </si>
   <si>
     <t>VERY IMPORTANT ARTICLE that makes the case for regulation.</t>
+  </si>
+  <si>
+    <t>ALL THE PAPER IS SUPER INTERESTING AND RELEVANT -&gt; "We analyze nine regulatory strategies that may help individuals avoid financial mistakes. We discuss laissez-faire, disclosure, nudges, financial “driver’s licenses,” advance directives, fiduciaries, asset safe harbors, and ex post and ex ante regulatory oversight. Finally, we pose seven questions for future research on cognitive limitations and associated policy responses."</t>
+  </si>
+  <si>
+    <t>Calls for policies but no examples and pretty vague in the conclusion.</t>
+  </si>
+  <si>
+    <t>No calls for policies, just an analysis.</t>
+  </si>
+  <si>
+    <t>Introduction -&gt; "We expect the determinants of information disclosure discussed above to play an important role also in:
+Labor relationships. An employer who hires a worker typically receives letters of recommendation from previous employers describing the worker’s characteristics (talent, fairness, relations with colleagues), but also the tasks performed in upstream relationships.
+Insurance. Clients who purchase multiple policies are notified that relevant personal information (e.g. the number of accidents in the past few years and the type of risk borne by policy-holders) will be shared with partners.
+Financial relationships. Venture capitalists often disclose information about a project’s profitability, as well as personal characteristics of entrepreneurs, to other investors in order to convince them to join. Entrants in the credit card market get detailed information on potential customers from credit bureaus and other lenders.
+Regulation and taxation of multinational firms. Foreign regulators usually operate on the basis of the information provided by domestic agencies. Information-sharing between domestic and foreign tax authorities is often considered to be largely strategic and is at the heart of political debates."
+Conclusion -&gt; "The design of optimal policies in environments where disclosure may be driven by a combination of the diﬀerent determinants discussed above is an interesting line for future research. Similarly, relaxing the assumption of full commitment may deliver new insights into the welfare eﬀects of disclosure and the desirability of regulatory intervention in the area of privacy. We expect the main strategic eﬀects that we have highlighted to prove useful also in the study of these more complex environments."</t>
+  </si>
+  <si>
+    <t>Introductiion and Conclusion face the topic -&gt; definitely a suggested reading.</t>
+  </si>
+  <si>
+    <t>ALL THE PAPER -&gt; "We show that policy intervention banning the collection of personally identifiable data (e.g., through stricter privacy laws requiring user consent) is beneficial when consumers are naïve, competition is limited, and firms can price discriminate. Otherwise, privacy regulation often backfires."</t>
+  </si>
+  <si>
+    <t>Might have good insights.</t>
+  </si>
+  <si>
+    <t>Something on price floors, but no focus.</t>
   </si>
 </sst>
 </file>
@@ -825,7 +851,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -847,6 +873,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -936,7 +968,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -965,9 +997,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1039,6 +1068,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1357,10 +1392,10 @@
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I53" sqref="I53"/>
+      <selection pane="bottomRight" activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1402,34 +1437,34 @@
       <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="153" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>2006</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="18" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="17" t="s">
         <v>216</v>
       </c>
     </row>
@@ -1446,7 +1481,7 @@
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>217</v>
       </c>
     </row>
@@ -1463,32 +1498,32 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="17"/>
+      <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:9" ht="119" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>2010</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="19" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="18" t="s">
         <v>219</v>
       </c>
     </row>
@@ -1505,7 +1540,7 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="19" t="s">
         <v>218</v>
       </c>
     </row>
@@ -1522,34 +1557,34 @@
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="19" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="153" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>2015</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="19" t="s">
+      <c r="H8" s="13"/>
+      <c r="I8" s="18" t="s">
         <v>222</v>
       </c>
     </row>
@@ -1568,32 +1603,32 @@
         <v>221</v>
       </c>
       <c r="H9" s="5"/>
-      <c r="I9" s="17"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>2007</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="18" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="17" t="s">
         <v>223</v>
       </c>
     </row>
@@ -1610,59 +1645,59 @@
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="17"/>
+      <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="170" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>2016</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="19" t="s">
+      <c r="H12" s="13"/>
+      <c r="I12" s="18" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="11">
         <v>2006</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="18" t="s">
+      <c r="H13" s="13"/>
+      <c r="I13" s="17" t="s">
         <v>223</v>
       </c>
     </row>
@@ -1679,7 +1714,7 @@
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="17"/>
+      <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
@@ -1694,59 +1729,59 @@
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="17"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="13">
         <v>2014</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="18" t="s">
+      <c r="H16" s="13"/>
+      <c r="I16" s="17" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <v>2015</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="18" t="s">
+      <c r="H17" s="13"/>
+      <c r="I17" s="17" t="s">
         <v>225</v>
       </c>
     </row>
@@ -1763,298 +1798,298 @@
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="16" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="153" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="13">
         <v>2004</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="18" t="s">
+      <c r="H19" s="13"/>
+      <c r="I19" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="13">
         <v>1997</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="18" t="s">
+      <c r="H20" s="13"/>
+      <c r="I20" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="13">
         <v>1999</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="I21" s="18" t="s">
+      <c r="I21" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="13">
         <v>2001</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="18" t="s">
+      <c r="H22" s="13"/>
+      <c r="I22" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="13">
         <v>1968</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13" t="s">
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="18" t="s">
+      <c r="H23" s="13"/>
+      <c r="I23" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="13">
         <v>2005</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13" t="s">
+      <c r="D24" s="12"/>
+      <c r="E24" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="18" t="s">
+      <c r="H24" s="13"/>
+      <c r="I24" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="13">
         <v>2006</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13" t="s">
+      <c r="D25" s="12"/>
+      <c r="E25" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="18" t="s">
+      <c r="H25" s="13"/>
+      <c r="I25" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="13">
         <v>2014</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13" t="s">
+      <c r="D26" s="12"/>
+      <c r="E26" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F26" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="18" t="s">
+      <c r="H26" s="13"/>
+      <c r="I26" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="13">
         <v>2014</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13" t="s">
+      <c r="D27" s="12"/>
+      <c r="E27" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="18" t="s">
+      <c r="H27" s="13"/>
+      <c r="I27" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="204" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="H28" s="14"/>
-      <c r="I28" s="19" t="s">
+      <c r="H28" s="13"/>
+      <c r="I28" s="18" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="340" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="11">
         <v>2012</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="H29" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="I29" s="18" t="s">
+      <c r="I29" s="17" t="s">
         <v>228</v>
       </c>
     </row>
@@ -2071,105 +2106,105 @@
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="20" t="s">
+      <c r="I30" s="19" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="13">
         <v>2011</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="18" t="s">
+      <c r="H31" s="13"/>
+      <c r="I31" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13" t="s">
+      <c r="D32" s="12"/>
+      <c r="E32" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="H32" s="14"/>
-      <c r="I32" s="18" t="s">
+      <c r="H32" s="13"/>
+      <c r="I32" s="17" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="13">
         <v>2009</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13" t="s">
+      <c r="D33" s="12"/>
+      <c r="E33" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="H33" s="14"/>
-      <c r="I33" s="18" t="s">
+      <c r="H33" s="13"/>
+      <c r="I33" s="17" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="13">
         <v>2008</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13" t="s">
+      <c r="D34" s="12"/>
+      <c r="E34" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="18" t="s">
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="17" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2186,772 +2221,802 @@
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="24" t="s">
+      <c r="I35" s="23" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="13">
         <v>2014</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="H36" s="14"/>
-      <c r="I36" s="20" t="s">
+      <c r="H36" s="13"/>
+      <c r="I36" s="19" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="13">
         <v>2009</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13" t="s">
+      <c r="D37" s="12"/>
+      <c r="E37" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="G37" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="H37" s="14"/>
-      <c r="I37" s="18" t="s">
+      <c r="H37" s="13"/>
+      <c r="I37" s="17" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="204" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="13">
         <v>2015</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="23" t="s">
+      <c r="D38" s="12"/>
+      <c r="E38" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="19" t="s">
+      <c r="H38" s="13"/>
+      <c r="I38" s="18" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="26">
+      <c r="B39" s="25">
         <v>2008</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="27" t="s">
+      <c r="D39" s="24"/>
+      <c r="E39" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="F39" s="26" t="s">
+      <c r="F39" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="G39" s="26" t="s">
+      <c r="G39" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="H39" s="26"/>
-      <c r="I39" s="28" t="s">
+      <c r="H39" s="25"/>
+      <c r="I39" s="27" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="26">
+      <c r="B40" s="25">
         <v>1991</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="D40" s="25"/>
-      <c r="E40" s="27" t="s">
+      <c r="D40" s="24"/>
+      <c r="E40" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="F40" s="26" t="s">
+      <c r="F40" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="G40" s="26" t="s">
+      <c r="G40" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="H40" s="26"/>
-      <c r="I40" s="33" t="s">
+      <c r="H40" s="25"/>
+      <c r="I40" s="32" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="30">
+      <c r="B41" s="29">
         <v>2010</v>
       </c>
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="31" t="s">
+      <c r="D41" s="28"/>
+      <c r="E41" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="F41" s="30" t="s">
+      <c r="F41" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="G41" s="30" t="s">
+      <c r="G41" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="H41" s="30"/>
-      <c r="I41" s="34" t="s">
+      <c r="H41" s="29"/>
+      <c r="I41" s="33" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="26">
+      <c r="B42" s="25">
         <v>2004</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="25"/>
-      <c r="E42" s="27" t="s">
+      <c r="D42" s="24"/>
+      <c r="E42" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="F42" s="26" t="s">
+      <c r="F42" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="G42" s="26" t="s">
+      <c r="G42" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="H42" s="26" t="s">
+      <c r="H42" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="I42" s="28" t="s">
+      <c r="I42" s="27" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="26">
+      <c r="B43" s="25">
         <v>1997</v>
       </c>
-      <c r="C43" s="25" t="s">
+      <c r="C43" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D43" s="25"/>
-      <c r="E43" s="27" t="s">
+      <c r="D43" s="24"/>
+      <c r="E43" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="F43" s="26" t="s">
+      <c r="F43" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="G43" s="26" t="s">
+      <c r="G43" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="H43" s="26"/>
-      <c r="I43" s="28" t="s">
+      <c r="H43" s="25"/>
+      <c r="I43" s="27" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="170" x14ac:dyDescent="0.2">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="26">
+      <c r="B44" s="25">
         <v>2008</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="27" t="s">
+      <c r="D44" s="24"/>
+      <c r="E44" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="F44" s="26" t="s">
+      <c r="F44" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="G44" s="26" t="s">
+      <c r="G44" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="H44" s="26"/>
-      <c r="I44" s="28" t="s">
+      <c r="H44" s="25"/>
+      <c r="I44" s="27" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="26">
+      <c r="B45" s="25">
         <v>2009</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="25"/>
-      <c r="E45" s="27" t="s">
+      <c r="D45" s="24"/>
+      <c r="E45" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="F45" s="26" t="s">
+      <c r="F45" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="G45" s="26" t="s">
+      <c r="G45" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="H45" s="26"/>
-      <c r="I45" s="28" t="s">
+      <c r="H45" s="25"/>
+      <c r="I45" s="27" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="221" x14ac:dyDescent="0.2">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D46" s="25" t="s">
+      <c r="D46" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="E46" s="25" t="s">
+      <c r="E46" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="F46" s="26" t="s">
+      <c r="F46" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="G46" s="26" t="s">
+      <c r="G46" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="H46" s="26"/>
-      <c r="I46" s="28" t="s">
+      <c r="H46" s="25"/>
+      <c r="I46" s="27" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C47" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D47" s="25" t="s">
+      <c r="D47" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="E47" s="25" t="s">
+      <c r="E47" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="F47" s="26" t="s">
+      <c r="F47" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="G47" s="26" t="s">
+      <c r="G47" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="H47" s="26"/>
-      <c r="I47" s="28" t="s">
+      <c r="H47" s="25"/>
+      <c r="I47" s="27" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="26">
+      <c r="B48" s="25">
         <v>2009</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25" t="s">
+      <c r="D48" s="24"/>
+      <c r="E48" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="F48" s="26" t="s">
+      <c r="F48" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="26" t="s">
+      <c r="G48" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="H48" s="26"/>
-      <c r="I48" s="33" t="s">
+      <c r="H48" s="25"/>
+      <c r="I48" s="32" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A49" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="25">
+        <v>2011</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="F49" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="G49" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="H49" s="25"/>
+      <c r="I49" s="27" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A49" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B49" s="26">
+    <row r="50" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A50" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="25">
+        <v>2008</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="F50" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="G50" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="H50" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I50" s="32" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A51" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="25">
+        <v>2007</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G51" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="H51" s="25"/>
+      <c r="I51" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A52" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="25">
+        <v>2010</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F52" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G52" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="H52" s="25"/>
+      <c r="I52" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A53" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="25">
+        <v>1920</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F53" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G53" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="H53" s="25"/>
+      <c r="I53" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A54" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="25">
+        <v>1933</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F54" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G54" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="H54" s="25"/>
+      <c r="I54" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A55" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="25">
+        <v>1980</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G55" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="H55" s="25"/>
+      <c r="I55" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A56" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="29">
+        <v>1981</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="F56" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="G56" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="H56" s="29"/>
+      <c r="I56" s="23" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A57" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F57" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G57" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="H57" s="25"/>
+      <c r="I57" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A58" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="25">
+        <v>2004</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F58" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G58" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="H58" s="25"/>
+      <c r="I58" s="27" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A59" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" s="25">
+        <v>2005</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F59" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G59" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="H59" s="25"/>
+      <c r="I59" s="27" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A60" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" s="25">
+        <v>2006</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F60" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G60" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="H60" s="25"/>
+      <c r="I60" s="27" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A61" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B61" s="25">
+        <v>2006</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G61" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="H61" s="25"/>
+      <c r="I61" s="27" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A62" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F62" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G62" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="H62" s="25"/>
+      <c r="I62" s="35" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A63" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="25">
         <v>2011</v>
       </c>
-      <c r="C49" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="F49" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="G49" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="H49" s="26"/>
-      <c r="I49" s="28" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A50" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B50" s="26">
+      <c r="C63" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="F63" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G63" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H63" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I63" s="27" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" s="25">
+        <v>2016</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="F64" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G64" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="H64" s="25"/>
+      <c r="I64" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A65" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" s="25">
         <v>2008</v>
       </c>
-      <c r="C50" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="F50" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="G50" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="H50" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="I50" s="33" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="119" x14ac:dyDescent="0.2">
-      <c r="A51" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" s="26">
-        <v>2007</v>
-      </c>
-      <c r="C51" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="F51" s="32" t="s">
+      <c r="C65" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F65" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="G51" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="H51" s="26"/>
-      <c r="I51" s="28" t="s">
+      <c r="G65" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="H65" s="25"/>
+      <c r="I65" s="27" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B52" s="5">
-        <v>2010</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="H52" s="5"/>
-      <c r="I52" s="17"/>
-    </row>
-    <row r="53" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B53" s="5">
-        <v>1920</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="H53" s="5"/>
-      <c r="I53" s="17"/>
-    </row>
-    <row r="54" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B54" s="5">
-        <v>1933</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="H54" s="5"/>
-      <c r="I54" s="17"/>
-    </row>
-    <row r="55" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B55" s="5">
-        <v>1980</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H55" s="5"/>
-      <c r="I55" s="17"/>
-    </row>
-    <row r="56" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B56" s="5">
-        <v>1981</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H56" s="5"/>
-      <c r="I56" s="17"/>
-    </row>
-    <row r="57" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H57" s="5"/>
-      <c r="I57" s="17"/>
-    </row>
-    <row r="58" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B58" s="5">
-        <v>2004</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H58" s="5"/>
-      <c r="I58" s="17"/>
-    </row>
-    <row r="59" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B59" s="5">
-        <v>2005</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H59" s="5"/>
-      <c r="I59" s="17"/>
-    </row>
-    <row r="60" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B60" s="5">
-        <v>2006</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H60" s="5"/>
-      <c r="I60" s="17"/>
-    </row>
-    <row r="61" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B61" s="5">
-        <v>2006</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F61" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H61" s="5"/>
-      <c r="I61" s="17"/>
-    </row>
-    <row r="62" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H62" s="5"/>
-      <c r="I62" s="17"/>
-    </row>
-    <row r="63" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B63" s="5">
-        <v>2011</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I63" s="17"/>
-    </row>
-    <row r="64" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B64" s="5">
-        <v>2016</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="H64" s="5"/>
-      <c r="I64" s="17"/>
-    </row>
-    <row r="65" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B65" s="5">
-        <v>2008</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="H65" s="5"/>
-      <c r="I65" s="17"/>
-    </row>
     <row r="66" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B66" s="25">
         <v>2015</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="E66" s="6" t="s">
+      <c r="E66" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="G66" s="5" t="s">
+      <c r="G66" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="H66" s="5"/>
-      <c r="I66" s="17"/>
+      <c r="H66" s="25"/>
+      <c r="I66" s="27" t="s">
+        <v>250</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>